<commit_message>
ETL pipeline now includes Region spreadsheet, required for #13
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2012_102112.xlsx
+++ b/data/GroupingsOBSQuestions2012_102112.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="-240" windowWidth="19160" windowHeight="13480"/>
+    <workbookView xWindow="300" yWindow="-240" windowWidth="19160" windowHeight="13540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionsGroups" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,226 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="159">
+  <si>
+    <t>United States</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Western Europe &amp; the U.S.</t>
+  </si>
+  <si>
+    <t>Sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>South Asia</t>
+  </si>
+  <si>
+    <t>Middle East &amp; North Africa</t>
+  </si>
+  <si>
+    <t>Latin America &amp; Caribbean</t>
+  </si>
+  <si>
+    <t>Eastern Europe &amp; Central Asia</t>
+  </si>
+  <si>
+    <t>East Asia &amp; Pacific</t>
+  </si>
+  <si>
+    <t>Countries grouped by Region (this can also be further disaggregated, but can we do this at a second stage?)</t>
+  </si>
+  <si>
+    <t>1-58</t>
+  </si>
+  <si>
+    <t>59, 97-100, 102-107</t>
+  </si>
+  <si>
+    <t>90, 92-94</t>
+  </si>
+  <si>
+    <t>Note that the numbers were different for 2010: there were more questions, but we realised that we were using the same questions twice (in the Audit Report sub index, and in the SAI strength, so we took some out, to avoid overlapping)</t>
+  </si>
+  <si>
+    <t>Info throughout all eight key documents</t>
+  </si>
+  <si>
+    <t>The Open Budget Questionnaire</t>
+  </si>
+  <si>
+    <t>59, 90, 92-94, 97-100, 102-107, 114-125</t>
+  </si>
+  <si>
+    <t>Info in the Executive's Budget Proposal:</t>
+  </si>
+  <si>
+    <t>1-58, 60-64, 66-71, 73-89, 91, 95-96, 101, 108-112</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Executive's Budget Proposal</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Pre-Budget Statement</t>
+  </si>
+  <si>
+    <t>In-Year Reports</t>
+  </si>
+  <si>
+    <t>Year-End Report</t>
+  </si>
+  <si>
+    <t>Audit Report</t>
+  </si>
+  <si>
+    <t>Citizens Budget</t>
+  </si>
+  <si>
+    <t>Mid-Year Review</t>
+  </si>
+  <si>
+    <t>Enacted Budget</t>
+  </si>
+  <si>
+    <t>77-86</t>
+  </si>
+  <si>
+    <t>73-76</t>
+  </si>
+  <si>
+    <t>The Open Budget Index</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oversight Questions</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Performance Information</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Honduras</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>63-72</t>
   </si>
@@ -49,9 +268,6 @@
     <t>(this includes info on expenditure, revenue and debt, so in principle it can be further disaggregated)</t>
   </si>
   <si>
-    <t>Performance Information (and policy-related)</t>
-  </si>
-  <si>
     <t>18-34</t>
   </si>
   <si>
@@ -73,9 +289,6 @@
     <t>16-17, 48-55, 83-85</t>
   </si>
   <si>
-    <t>Performance Information (and policy related)</t>
-  </si>
-  <si>
     <t>By Key Budget Document</t>
   </si>
   <si>
@@ -202,9 +415,6 @@
     <t>Liberia</t>
   </si>
   <si>
-    <t>Honduras</t>
-  </si>
-  <si>
     <t>Poland</t>
   </si>
   <si>
@@ -224,9 +434,6 @@
   </si>
   <si>
     <t>Philippines</t>
-  </si>
-  <si>
-    <t>United States</t>
   </si>
   <si>
     <t>Ghana</t>
@@ -298,211 +505,6 @@
   </si>
   <si>
     <t>Morocco</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Mongolia</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Croatia</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Burkina Faso</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Iraq</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t>Fiji</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Benin</t>
-  </si>
-  <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>Azerbaijan</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Angola</t>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
-    <t>Algeria</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Albania</t>
-  </si>
-  <si>
-    <t>Cambodia</t>
-  </si>
-  <si>
-    <t>Western Europe &amp; the U.S.</t>
-  </si>
-  <si>
-    <t>Sub-Saharan Africa</t>
-  </si>
-  <si>
-    <t>South Asia</t>
-  </si>
-  <si>
-    <t>Middle East &amp; North Africa</t>
-  </si>
-  <si>
-    <t>Latin America &amp; Caribbean</t>
-  </si>
-  <si>
-    <t>Eastern Europe &amp; Central Asia</t>
-  </si>
-  <si>
-    <t>East Asia &amp; Pacific</t>
-  </si>
-  <si>
-    <t>Countries grouped by Region (this can also be further disaggregated, but can we do this at a second stage?)</t>
-  </si>
-  <si>
-    <t>1-58</t>
-  </si>
-  <si>
-    <t>59, 97-100, 102-107</t>
-  </si>
-  <si>
-    <t>90, 92-94</t>
-  </si>
-  <si>
-    <t>Note that the numbers were different for 2010: there were more questions, but we realised that we were using the same questions twice (in the Audit Report sub index, and in the SAI strength, so we took some out, to avoid overlapping)</t>
-  </si>
-  <si>
-    <t>Info throughout all eight key documents</t>
-  </si>
-  <si>
-    <t>The Open Budget Questionnaire</t>
-  </si>
-  <si>
-    <t>Transparency Questions (the Open Budget Index)</t>
-  </si>
-  <si>
-    <t>Oversight Questions (SAI, Legislature and Public)</t>
-  </si>
-  <si>
-    <t>59, 90, 92-94, 97-100, 102-107, 114-125</t>
-  </si>
-  <si>
-    <t>Info in the Executive's Budget Proposal:</t>
-  </si>
-  <si>
-    <t>1-58, 60-64, 66-71, 73-89, 91, 95-96, 101, 108-112</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Executive's Budget Proposal</t>
-  </si>
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
-    <t>Pre-Budget Statement</t>
-  </si>
-  <si>
-    <t>In-Year Reports</t>
-  </si>
-  <si>
-    <t>Year-End Report</t>
-  </si>
-  <si>
-    <t>Audit Report</t>
-  </si>
-  <si>
-    <t>Citizens Budget</t>
-  </si>
-  <si>
-    <t>Mid-Year Review</t>
-  </si>
-  <si>
-    <t>Enacted Budget</t>
-  </si>
-  <si>
-    <t>77-86</t>
-  </si>
-  <si>
-    <t>73-76</t>
   </si>
 </sst>
 </file>
@@ -903,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -917,7 +919,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="7" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="7"/>
@@ -925,18 +927,18 @@
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>144</v>
+      <c r="B4" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>148</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -944,15 +946,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="3" t="s">
-        <v>147</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -960,16 +962,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -977,16 +979,16 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -994,32 +996,32 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1027,10 +1029,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>139</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1038,13 +1040,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>141</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1052,18 +1054,18 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1071,10 +1073,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>151</v>
+        <v>58</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1082,10 +1084,10 @@
         <v>2</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1093,7 +1095,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>157</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2">
         <v>101</v>
@@ -1104,10 +1106,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1115,10 +1117,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1126,10 +1128,10 @@
         <v>6</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>153</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>158</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1137,10 +1139,10 @@
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>154</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1148,15 +1150,15 @@
         <v>8</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>155</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="3" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1164,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1175,10 +1177,10 @@
         <v>2</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1186,10 +1188,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1197,13 +1199,14 @@
         <v>4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1218,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1236,7 +1239,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19">
       <c r="A1" s="9" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1247,385 +1250,386 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>126</v>
+        <v>35</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>122</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" s="5" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="F23" s="5" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="F24" s="5" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="F25" s="5" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="F26" s="5" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="F27" s="5" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="F28" s="5" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="F29" s="5" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="F30" s="5" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>